<commit_message>
feat: completed case study for Course 1 Module 2
</commit_message>
<xml_diff>
--- a/excel-basics/formula/notes.xlsx
+++ b/excel-basics/formula/notes.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\power-bi-cert\excel-basics\formula\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739D4B37-89DE-4C62-AEF5-B678BBD3F55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B602F140-394C-4894-9050-08C1AA1A3BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0D076788-1608-43AF-9E52-FBAA486EFBE6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{0D076788-1608-43AF-9E52-FBAA486EFBE6}"/>
   </bookViews>
   <sheets>
     <sheet name="chaining calculations" sheetId="1" r:id="rId1"/>
     <sheet name="link calculation" sheetId="2" r:id="rId2"/>
+    <sheet name="cell reference" sheetId="3" r:id="rId3"/>
+    <sheet name="aboslute reference syntax" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -375,17 +377,293 @@
         </r>
       </text>
     </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{DF75D6CB-5BE1-4DAB-AEE5-D5C2931FD6A3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Asus:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+to use exponents:
+&lt;value&gt;^power
+it's just using the ^ symbol</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Asus</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{84AB4191-7777-47A6-B055-16D507050C3B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Asus:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Logical operations </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">return </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>boolean</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> values
+In this case, =C2&gt;3
+since value in C2, 4 &gt; 3, the value is true.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{B12C7F93-EB6A-4DDD-8D2E-37DA6199B625}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Asus:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Use </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">dollar sign, $ </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">to signify a constant value
+$J2 + $K2 keeps ensures the formula always refers to columns J2 and K2 and onwards for values.
+This is important for values such as </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> excahnge rates</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Asus</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{1EEB2787-46E3-4146-9C8C-930E1D2786B9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Asus:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+How the absolute reference syntax is used can affect the outcome.
+Check note: </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Relative and Absolute Cell References for more details</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{ED0FEDDF-BA90-40FE-8179-7895E3877672}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">To get percentage </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(in growth in this case):
+1. =(G1-F1)/G1
+2. Convert H to percentage
+3. In order to use autofill on current col, there must be data in the col to the left of cur col, hence why column E is needed.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+  <si>
+    <t>rel 1</t>
+  </si>
+  <si>
+    <t>rel 2</t>
+  </si>
+  <si>
+    <t>rel3</t>
+  </si>
+  <si>
+    <t>rel4</t>
+  </si>
+  <si>
+    <t>out1</t>
+  </si>
+  <si>
+    <t>out2</t>
+  </si>
+  <si>
+    <t>ab1</t>
+  </si>
+  <si>
+    <t>ab2</t>
+  </si>
+  <si>
+    <t>ab3</t>
+  </si>
+  <si>
+    <t>ab4</t>
+  </si>
+  <si>
+    <t>$C$3</t>
+  </si>
+  <si>
+    <t>$C3</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +697,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -428,7 +721,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -436,16 +729,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -921,183 +1236,597 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBDFFFD1-5016-4BC7-BE09-0FFC88DCBD02}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <f>A1*'chaining calculations'!G1</f>
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
+        <f>'chaining calculations'!E1+'chaining calculations'!G1</f>
+        <v>6</v>
+      </c>
+      <c r="F1">
+        <f>'chaining calculations'!G1+B1</f>
+        <v>8</v>
+      </c>
+      <c r="G1">
+        <f>F1^3</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <f>A2*'chaining calculations'!G2</f>
+        <v>24</v>
+      </c>
+      <c r="E2" s="1">
+        <f>'chaining calculations'!E2+'chaining calculations'!G2</f>
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <f>'chaining calculations'!G2+B2</f>
+        <v>36</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G10" si="0">F2^3</f>
+        <v>46656</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <f>A3*'chaining calculations'!G3</f>
+        <v>72</v>
+      </c>
+      <c r="E3" s="1">
+        <f>'chaining calculations'!E3+'chaining calculations'!G3</f>
+        <v>36</v>
+      </c>
+      <c r="F3">
+        <f>'chaining calculations'!G3+B3</f>
+        <v>96</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>884736</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f>A4*'chaining calculations'!G4</f>
+        <v>160</v>
+      </c>
+      <c r="E4" s="1">
+        <f>'chaining calculations'!E4+'chaining calculations'!G4</f>
+        <v>60</v>
+      </c>
+      <c r="F4">
+        <f>'chaining calculations'!G4+B4</f>
+        <v>200</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <f>A5*'chaining calculations'!G5</f>
+        <v>300</v>
+      </c>
+      <c r="E5" s="1">
+        <f>'chaining calculations'!E5+'chaining calculations'!G5</f>
+        <v>90</v>
+      </c>
+      <c r="F5">
+        <f>'chaining calculations'!G5+B5</f>
+        <v>360</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>46656000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f>A6*'chaining calculations'!G6</f>
+        <v>504</v>
+      </c>
+      <c r="E6" s="1">
+        <f>'chaining calculations'!E6+'chaining calculations'!G6</f>
+        <v>126</v>
+      </c>
+      <c r="F6">
+        <f>'chaining calculations'!G6+B6</f>
+        <v>588</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>203297472</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <f>A7*'chaining calculations'!G7</f>
+        <v>784</v>
+      </c>
+      <c r="E7" s="1">
+        <f>'chaining calculations'!E7+'chaining calculations'!G7</f>
+        <v>168</v>
+      </c>
+      <c r="F7">
+        <f>'chaining calculations'!G7+B7</f>
+        <v>896</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>719323136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <f>A8*'chaining calculations'!G8</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <f>'chaining calculations'!E8+'chaining calculations'!G8</f>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f>'chaining calculations'!G8+B8</f>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <f>A9*'chaining calculations'!G9</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <f>'chaining calculations'!E9+'chaining calculations'!G9</f>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f>'chaining calculations'!G9+B9</f>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <f>A10*'chaining calculations'!G10</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <f>'chaining calculations'!E10+'chaining calculations'!G10</f>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f>'chaining calculations'!G10+B10</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6906624-BC12-400D-B071-B5D66958F680}">
+  <dimension ref="A1:P3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
-        <f>A1*'chaining calculations'!G1</f>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1">
-        <f>'chaining calculations'!E1+'chaining calculations'!G1</f>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <f>A2+B2</f>
+        <v>4</v>
+      </c>
+      <c r="D2" t="b">
+        <f>C2&gt;3</f>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <f>F2+G2</f>
+        <v>12</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <f>$J2+$K2</f>
+        <v>4</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>7</v>
+      </c>
+      <c r="P2">
+        <f>$J2+$K2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <f>A3+B3</f>
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <f>F3+G3</f>
+        <v>14</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <f>$J3+$K3</f>
+        <v>6</v>
+      </c>
+      <c r="N3">
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <f>$J3+$K3</f>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FC3591-ECA8-47B5-BAD3-CAA361E8773A}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
       <c r="F1">
-        <f>'chaining calculations'!G1+B1</f>
+        <v>2</v>
+      </c>
+      <c r="G1">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4">
+        <f>(G1-F1)/G1</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <f>$C$2</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <f>$C3</f>
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2" s="4">
+        <f t="shared" ref="H2:H7" si="0">(G2-F2)/G2</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <f>$C$2</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <f t="shared" ref="B3:B10" si="1">$C4</f>
+        <v>3</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <f>$C$2</f>
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <f>$C$2</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <f>$C$2</f>
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <f>A2*'chaining calculations'!G2</f>
-        <v>24</v>
-      </c>
-      <c r="E2" s="1">
-        <f>'chaining calculations'!E2+'chaining calculations'!G2</f>
-        <v>18</v>
-      </c>
-      <c r="F2">
-        <f>'chaining calculations'!G2+B2</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <f>A3*'chaining calculations'!G3</f>
-        <v>72</v>
-      </c>
-      <c r="E3" s="1">
-        <f>'chaining calculations'!E3+'chaining calculations'!G3</f>
-        <v>36</v>
-      </c>
-      <c r="F3">
-        <f>'chaining calculations'!G3+B3</f>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <f>A4*'chaining calculations'!G4</f>
-        <v>160</v>
-      </c>
-      <c r="E4" s="1">
-        <f>'chaining calculations'!E4+'chaining calculations'!G4</f>
-        <v>60</v>
-      </c>
-      <c r="F4">
-        <f>'chaining calculations'!G4+B4</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <f>A5*'chaining calculations'!G5</f>
-        <v>300</v>
-      </c>
-      <c r="E5" s="1">
-        <f>'chaining calculations'!E5+'chaining calculations'!G5</f>
-        <v>90</v>
-      </c>
-      <c r="F5">
-        <f>'chaining calculations'!G5+B5</f>
-        <v>360</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="H6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <f>$C$2</f>
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
         <v>6</v>
       </c>
-      <c r="B6">
-        <f>A6*'chaining calculations'!G6</f>
-        <v>504</v>
-      </c>
-      <c r="E6" s="1">
-        <f>'chaining calculations'!E6+'chaining calculations'!G6</f>
-        <v>126</v>
-      </c>
-      <c r="F6">
-        <f>'chaining calculations'!G6+B6</f>
-        <v>588</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="E7">
         <v>7</v>
       </c>
-      <c r="B7">
-        <f>A7*'chaining calculations'!G7</f>
-        <v>784</v>
-      </c>
-      <c r="E7" s="1">
-        <f>'chaining calculations'!E7+'chaining calculations'!G7</f>
-        <v>168</v>
-      </c>
       <c r="F7">
-        <f>'chaining calculations'!G7+B7</f>
-        <v>896</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8">
-        <f>A8*'chaining calculations'!G8</f>
+      <c r="G7">
+        <v>9</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <f>$C$2</f>
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="1">
-        <f>'chaining calculations'!E8+'chaining calculations'!G8</f>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <f>$C$2</f>
+        <v>1</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8">
-        <f>'chaining calculations'!G8+B8</f>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <f>$C$2</f>
+        <v>1</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <f>A9*'chaining calculations'!G9</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <f>'chaining calculations'!E9+'chaining calculations'!G9</f>
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <f>'chaining calculations'!G9+B9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <f>A10*'chaining calculations'!G10</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <f>'chaining calculations'!E10+'chaining calculations'!G10</f>
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <f>'chaining calculations'!G10+B10</f>
-        <v>0</v>
-      </c>
+      <c r="C10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>